<commit_message>
add excel data ingester and update data in xlsx file
</commit_message>
<xml_diff>
--- a/example-data/salesdata-ca.xlsx
+++ b/example-data/salesdata-ca.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federico/dataprepml-java/ingest/wired-brain-coffee/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\machine-learning\machine-learning-data-ingestion\example-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE25601E-360A-8A4E-A5B8-9552DB06EFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516931C7-8636-43D9-81CF-0865CD296BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$B$1:$B$101</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="228">
   <si>
     <t>transaction_id</t>
   </si>
@@ -584,13 +587,133 @@
   </si>
   <si>
     <t>08/23/2020 02:32:39</t>
+  </si>
+  <si>
+    <t>08/05/2020  02:17:29</t>
+  </si>
+  <si>
+    <t>08/08/2020  12:33:29</t>
+  </si>
+  <si>
+    <t>08/08/2020  09:14:44</t>
+  </si>
+  <si>
+    <t>08/10/2020  02:14:24</t>
+  </si>
+  <si>
+    <t>08/03/2020  01:04:54</t>
+  </si>
+  <si>
+    <t>08/06/2020  02:05:20</t>
+  </si>
+  <si>
+    <t>08/11/2020  04:53:57</t>
+  </si>
+  <si>
+    <t>08/06/2020  05:31:56</t>
+  </si>
+  <si>
+    <t>08/08/2020  09:29:15</t>
+  </si>
+  <si>
+    <t>08/10/2020  05:40:14</t>
+  </si>
+  <si>
+    <t>08/10/2020  03:11:08</t>
+  </si>
+  <si>
+    <t>08/05/2020  09:35:30</t>
+  </si>
+  <si>
+    <t>08/05/2020  08:53:32</t>
+  </si>
+  <si>
+    <t>08/01/2020  03:27:59</t>
+  </si>
+  <si>
+    <t>08/05/2020  03:39:41</t>
+  </si>
+  <si>
+    <t>08/06/2020  11:19:42</t>
+  </si>
+  <si>
+    <t>08/02/2020  01:33:35</t>
+  </si>
+  <si>
+    <t>08/04/2020  05:01:21</t>
+  </si>
+  <si>
+    <t>08/11/2020  08:12:19</t>
+  </si>
+  <si>
+    <t>08/05/2020  11:59:05</t>
+  </si>
+  <si>
+    <t>08/08/2020  08:39:19</t>
+  </si>
+  <si>
+    <t>08/06/2020  09:44:47</t>
+  </si>
+  <si>
+    <t>08/08/2020  09:37:02</t>
+  </si>
+  <si>
+    <t>08/05/2020  02:24:28</t>
+  </si>
+  <si>
+    <t>08/08/2020  12:05:04</t>
+  </si>
+  <si>
+    <t>08/08/2020  03:00:53</t>
+  </si>
+  <si>
+    <t>08/08/2020  01:00:16</t>
+  </si>
+  <si>
+    <t>08/11/2020  07:05:05</t>
+  </si>
+  <si>
+    <t>08/08/2020  07:27:56</t>
+  </si>
+  <si>
+    <t>08/03/2020  03:13:27</t>
+  </si>
+  <si>
+    <t>08/08/2020  11:30:07</t>
+  </si>
+  <si>
+    <t>08/12/2020  11:11:34</t>
+  </si>
+  <si>
+    <t>08/11/2020  12:53:58</t>
+  </si>
+  <si>
+    <t>08/12/2020  08:14:06</t>
+  </si>
+  <si>
+    <t>08/08/2020  11:33:34</t>
+  </si>
+  <si>
+    <t>08/04/2020  05:32:15</t>
+  </si>
+  <si>
+    <t>08/10/2020  01:57:05</t>
+  </si>
+  <si>
+    <t>08/06/2020  12:56:54</t>
+  </si>
+  <si>
+    <t>08/08/2020  05:03:22</t>
+  </si>
+  <si>
+    <t>08/01/2020  11:56:07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -601,6 +724,13 @@
       <name val="DFGGiHi-W7"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -623,12 +753,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,9 +776,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +816,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -790,7 +922,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -942,26 +1074,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="256" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="256" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -987,8 +1119,8 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>43959.09547453704</v>
+      <c r="B2" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="C2" t="s">
         <v>124</v>
@@ -1013,7 +1145,7 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C3" t="s">
@@ -1036,8 +1168,8 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1">
-        <v>44051.523252314815</v>
+      <c r="B4" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="C4" t="s">
         <v>126</v>
@@ -1056,8 +1188,8 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1">
-        <v>44051.385231481479</v>
+      <c r="B5" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="C5" t="s">
         <v>127</v>
@@ -1079,8 +1211,8 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1">
-        <v>44112.093333333331</v>
+      <c r="B6" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>125</v>
@@ -1099,7 +1231,7 @@
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C7" t="s">
@@ -1119,7 +1251,7 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C8" t="s">
@@ -1139,7 +1271,7 @@
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C9" t="s">
@@ -1159,7 +1291,7 @@
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>151</v>
       </c>
       <c r="C10" t="s">
@@ -1179,7 +1311,7 @@
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C11" t="s">
@@ -1199,7 +1331,7 @@
       <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C12" t="s">
@@ -1225,7 +1357,7 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C13" t="s">
@@ -1248,7 +1380,7 @@
       <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C14" t="s">
@@ -1268,7 +1400,7 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C15" t="s">
@@ -1291,7 +1423,7 @@
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C16" t="s">
@@ -1314,7 +1446,7 @@
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>158</v>
       </c>
       <c r="C17" t="s">
@@ -1334,7 +1466,7 @@
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C18" t="s">
@@ -1354,7 +1486,7 @@
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>160</v>
       </c>
       <c r="C19" t="s">
@@ -1377,8 +1509,8 @@
       <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1">
-        <v>43898.045069444444</v>
+      <c r="B20" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="C20" t="s">
         <v>126</v>
@@ -1400,7 +1532,7 @@
       <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>161</v>
       </c>
       <c r="C21" t="s">
@@ -1420,7 +1552,7 @@
       <c r="A22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C22" t="s">
@@ -1440,7 +1572,7 @@
       <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>163</v>
       </c>
       <c r="C23" t="s">
@@ -1463,7 +1595,7 @@
       <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C24" t="s">
@@ -1486,8 +1618,8 @@
       <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="1">
-        <v>43990.087037037039</v>
+      <c r="B25" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="C25" t="s">
         <v>125</v>
@@ -1506,7 +1638,7 @@
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C26" t="s">
@@ -1529,7 +1661,7 @@
       <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>166</v>
       </c>
       <c r="C27" t="s">
@@ -1552,8 +1684,8 @@
       <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="1">
-        <v>44143.204131944447</v>
+      <c r="B28" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="C28" t="s">
         <v>125</v>
@@ -1572,7 +1704,7 @@
       <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C29" t="s">
@@ -1592,7 +1724,7 @@
       <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C30" t="s">
@@ -1612,7 +1744,7 @@
       <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C31" t="s">
@@ -1632,8 +1764,8 @@
       <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="1">
-        <v>43990.230509259258</v>
+      <c r="B32" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="C32" t="s">
         <v>124</v>
@@ -1655,7 +1787,7 @@
       <c r="A33" t="s">
         <v>54</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C33" t="s">
@@ -1678,7 +1810,7 @@
       <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>171</v>
       </c>
       <c r="C34" t="s">
@@ -1698,7 +1830,7 @@
       <c r="A35" t="s">
         <v>56</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C35" t="s">
@@ -1721,7 +1853,7 @@
       <c r="A36" t="s">
         <v>57</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>173</v>
       </c>
       <c r="C36" t="s">
@@ -1744,7 +1876,7 @@
       <c r="A37" t="s">
         <v>59</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>174</v>
       </c>
       <c r="C37" t="s">
@@ -1767,8 +1899,8 @@
       <c r="A38" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="1">
-        <v>44051.395312499997</v>
+      <c r="B38" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="C38" t="s">
         <v>125</v>
@@ -1790,7 +1922,7 @@
       <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>175</v>
       </c>
       <c r="C39" t="s">
@@ -1810,7 +1942,7 @@
       <c r="A40" t="s">
         <v>62</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>176</v>
       </c>
       <c r="C40" t="s">
@@ -1833,7 +1965,7 @@
       <c r="A41" t="s">
         <v>63</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C41" t="s">
@@ -1853,8 +1985,8 @@
       <c r="A42" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="1">
-        <v>44112.236273148148</v>
+      <c r="B42" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="C42" t="s">
         <v>127</v>
@@ -1876,8 +2008,8 @@
       <c r="A43" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="1">
-        <v>44112.132731481484</v>
+      <c r="B43" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="C43" t="s">
         <v>124</v>
@@ -1899,7 +2031,7 @@
       <c r="A44" t="s">
         <v>66</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C44" t="s">
@@ -1925,8 +2057,8 @@
       <c r="A45" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="1">
-        <v>43959.399652777778</v>
+      <c r="B45" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C45" t="s">
         <v>126</v>
@@ -1948,7 +2080,7 @@
       <c r="A46" t="s">
         <v>68</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C46" t="s">
@@ -1971,8 +2103,8 @@
       <c r="A47" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="1">
-        <v>43959.370509259257</v>
+      <c r="B47" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="C47" t="s">
         <v>127</v>
@@ -1994,8 +2126,8 @@
       <c r="A48" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="1">
-        <v>43838.144432870373</v>
+      <c r="B48" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="C48" t="s">
         <v>124</v>
@@ -2017,8 +2149,8 @@
       <c r="A49" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="1">
-        <v>43959.152557870373</v>
+      <c r="B49" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="C49" t="s">
         <v>125</v>
@@ -2037,8 +2169,8 @@
       <c r="A50" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="1">
-        <v>43990.472013888888</v>
+      <c r="B50" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="C50" t="s">
         <v>124</v>
@@ -2057,8 +2189,8 @@
       <c r="A51" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="1">
-        <v>43869.064988425926</v>
+      <c r="B51" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C51" t="s">
         <v>126</v>
@@ -2077,7 +2209,7 @@
       <c r="A52" t="s">
         <v>74</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C52" t="s">
@@ -2100,7 +2232,7 @@
       <c r="A53" t="s">
         <v>75</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>181</v>
       </c>
       <c r="C53" t="s">
@@ -2123,8 +2255,8 @@
       <c r="A54" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="1">
-        <v>43929.209270833337</v>
+      <c r="B54" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="C54" t="s">
         <v>124</v>
@@ -2146,8 +2278,8 @@
       <c r="A55" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="1">
-        <v>44143.341886574075</v>
+      <c r="B55" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="C55" t="s">
         <v>127</v>
@@ -2172,7 +2304,7 @@
       <c r="A56" t="s">
         <v>78</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>182</v>
       </c>
       <c r="C56" t="s">
@@ -2195,7 +2327,7 @@
       <c r="A57" t="s">
         <v>79</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>183</v>
       </c>
       <c r="C57" t="s">
@@ -2215,7 +2347,7 @@
       <c r="A58" t="s">
         <v>80</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>184</v>
       </c>
       <c r="C58" t="s">
@@ -2235,7 +2367,7 @@
       <c r="A59" t="s">
         <v>81</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>185</v>
       </c>
       <c r="C59" t="s">
@@ -2255,7 +2387,7 @@
       <c r="A60" t="s">
         <v>82</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C60" t="s">
@@ -2275,7 +2407,7 @@
       <c r="A61" t="s">
         <v>83</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C61" t="s">
@@ -2298,8 +2430,8 @@
       <c r="A62" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="1">
-        <v>43959.499363425923</v>
+      <c r="B62" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="C62" t="s">
         <v>127</v>
@@ -2321,7 +2453,7 @@
       <c r="A63" t="s">
         <v>85</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C63" t="s">
@@ -2344,7 +2476,7 @@
       <c r="A64" t="s">
         <v>86</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C64" t="s">
@@ -2367,8 +2499,8 @@
       <c r="A65" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="1">
-        <v>44051.360636574071</v>
+      <c r="B65" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="C65" t="s">
         <v>126</v>
@@ -2387,7 +2519,7 @@
       <c r="A66" t="s">
         <v>88</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C66" t="s">
@@ -2413,8 +2545,8 @@
       <c r="A67" t="s">
         <v>89</v>
       </c>
-      <c r="B67" s="1">
-        <v>43990.406099537038</v>
+      <c r="B67" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="C67" t="s">
         <v>126</v>
@@ -2433,7 +2565,7 @@
       <c r="A68" t="s">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C68" t="s">
@@ -2453,8 +2585,8 @@
       <c r="A69" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="1">
-        <v>44051.400717592594</v>
+      <c r="B69" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="C69" t="s">
         <v>124</v>
@@ -2473,8 +2605,8 @@
       <c r="A70" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="1">
-        <v>43959.100324074076</v>
+      <c r="B70" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C70" t="s">
         <v>127</v>
@@ -2493,8 +2625,8 @@
       <c r="A71" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="1">
-        <v>44051.503518518519</v>
+      <c r="B71" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="C71" t="s">
         <v>124</v>
@@ -2513,7 +2645,7 @@
       <c r="A72" t="s">
         <v>94</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C72" t="s">
@@ -2536,7 +2668,7 @@
       <c r="A73" t="s">
         <v>95</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C73" t="s">
@@ -2559,7 +2691,7 @@
       <c r="A74" t="s">
         <v>96</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C74" t="s">
@@ -2582,8 +2714,8 @@
       <c r="A75" t="s">
         <v>97</v>
       </c>
-      <c r="B75" s="1">
-        <v>44051.125613425924</v>
+      <c r="B75" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="C75" t="s">
         <v>127</v>
@@ -2605,7 +2737,7 @@
       <c r="A76" t="s">
         <v>98</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C76" t="s">
@@ -2631,7 +2763,7 @@
       <c r="A77" t="s">
         <v>99</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C77" t="s">
@@ -2654,7 +2786,7 @@
       <c r="A78" t="s">
         <v>100</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C78" t="s">
@@ -2677,8 +2809,8 @@
       <c r="A79" t="s">
         <v>101</v>
       </c>
-      <c r="B79" s="1">
-        <v>44051.041851851849</v>
+      <c r="B79" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C79" t="s">
         <v>127</v>
@@ -2697,8 +2829,8 @@
       <c r="A80" t="s">
         <v>102</v>
       </c>
-      <c r="B80" s="1">
-        <v>44143.29519675926</v>
+      <c r="B80" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="C80" t="s">
         <v>125</v>
@@ -2717,8 +2849,8 @@
       <c r="A81" t="s">
         <v>103</v>
       </c>
-      <c r="B81" s="1">
-        <v>44051.311064814814</v>
+      <c r="B81" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="C81" t="s">
         <v>126</v>
@@ -2737,8 +2869,8 @@
       <c r="A82" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="1">
-        <v>43898.134340277778</v>
+      <c r="B82" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="C82" t="s">
         <v>126</v>
@@ -2763,8 +2895,8 @@
       <c r="A83" t="s">
         <v>105</v>
       </c>
-      <c r="B83" s="1">
-        <v>44051.479247685187</v>
+      <c r="B83" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C83" t="s">
         <v>126</v>
@@ -2789,7 +2921,7 @@
       <c r="A84" t="s">
         <v>106</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C84" t="s">
@@ -2812,8 +2944,8 @@
       <c r="A85" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="1">
-        <v>44173.466365740744</v>
+      <c r="B85" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C85" t="s">
         <v>126</v>
@@ -2835,8 +2967,8 @@
       <c r="A86" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="1">
-        <v>44143.537476851852</v>
+      <c r="B86" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="C86" t="s">
         <v>126</v>
@@ -2861,8 +2993,8 @@
       <c r="A87" t="s">
         <v>109</v>
       </c>
-      <c r="B87" s="1">
-        <v>44173.343124999999</v>
+      <c r="B87" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="C87" t="s">
         <v>126</v>
@@ -2884,7 +3016,7 @@
       <c r="A88" t="s">
         <v>110</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C88" t="s">
@@ -2907,7 +3039,7 @@
       <c r="A89" t="s">
         <v>111</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C89" t="s">
@@ -2927,7 +3059,7 @@
       <c r="A90" t="s">
         <v>112</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C90" t="s">
@@ -2947,7 +3079,7 @@
       <c r="A91" t="s">
         <v>113</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>142</v>
       </c>
       <c r="C91" t="s">
@@ -2967,7 +3099,7 @@
       <c r="A92" t="s">
         <v>114</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C92" t="s">
@@ -2990,7 +3122,7 @@
       <c r="A93" t="s">
         <v>115</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C93" t="s">
@@ -3010,8 +3142,8 @@
       <c r="A94" t="s">
         <v>116</v>
       </c>
-      <c r="B94" s="1">
-        <v>44051.48164351852</v>
+      <c r="B94" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="C94" t="s">
         <v>125</v>
@@ -3030,8 +3162,8 @@
       <c r="A95" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="1">
-        <v>43929.230729166666</v>
+      <c r="B95" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="C95" t="s">
         <v>126</v>
@@ -3053,7 +3185,7 @@
       <c r="A96" t="s">
         <v>118</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C96" t="s">
@@ -3079,8 +3211,8 @@
       <c r="A97" t="s">
         <v>119</v>
       </c>
-      <c r="B97" s="1">
-        <v>44112.081307870372</v>
+      <c r="B97" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="C97" t="s">
         <v>127</v>
@@ -3102,8 +3234,8 @@
       <c r="A98" t="s">
         <v>120</v>
       </c>
-      <c r="B98" s="1">
-        <v>43990.539513888885</v>
+      <c r="B98" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="C98" t="s">
         <v>124</v>
@@ -3122,8 +3254,8 @@
       <c r="A99" t="s">
         <v>121</v>
       </c>
-      <c r="B99" s="1">
-        <v>44051.2106712963</v>
+      <c r="B99" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="C99" t="s">
         <v>124</v>
@@ -3145,7 +3277,7 @@
       <c r="A100" t="s">
         <v>122</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C100" t="s">
@@ -3168,8 +3300,8 @@
       <c r="A101" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="1">
-        <v>43838.497303240743</v>
+      <c r="B101" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="C101" t="s">
         <v>127</v>
@@ -3191,7 +3323,7 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
     <ignoredError sqref="G2" numberStoredAsText="1"/>

</xml_diff>